<commit_message>
some changes to the ski model + the PCA code
</commit_message>
<xml_diff>
--- a/SoothSkiSkiData.xlsx
+++ b/SoothSkiSkiData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\draga\Desktop\2.156 Code\Ski Project\Ski-Optimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laSch\Desktop\Fall 2025\2.156\Final Project\Code\Ski-Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FEAE5D3-A51F-4E9C-AB3F-FAEB5C8FF2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C2C4A7-6B78-4B65-8DEB-2A81BEB88D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2130" windowWidth="21600" windowHeight="11295" xr2:uid="{477FD795-673D-4956-B9BA-4D81E4004918}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{477FD795-673D-4956-B9BA-4D81E4004918}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -869,7 +869,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -989,12 +989,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1016,7 +1010,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1024,7 +1024,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{24764E70-367B-4108-B687-1B4D968491F4}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1355,106 +1357,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC9BA76-05BC-4CB0-B325-D49B2A1F79A2}">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="151.19999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AD1" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AE1" s="9" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1518,19 +1520,19 @@
       <c r="U2" s="2">
         <v>158</v>
       </c>
-      <c r="V2" s="12">
+      <c r="V2" s="10">
         <v>192</v>
       </c>
-      <c r="W2" s="12">
+      <c r="W2" s="10">
         <v>187</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="10">
         <v>166</v>
       </c>
-      <c r="Y2" s="12">
+      <c r="Y2" s="10">
         <v>170</v>
       </c>
-      <c r="Z2" s="12">
+      <c r="Z2" s="10">
         <v>177</v>
       </c>
       <c r="AA2" s="2">
@@ -1549,7 +1551,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1611,19 +1613,19 @@
       <c r="U3" s="2">
         <v>157.9</v>
       </c>
-      <c r="V3" s="12">
+      <c r="V3" s="10">
         <v>191.3</v>
       </c>
-      <c r="W3" s="12">
+      <c r="W3" s="10">
         <v>186.5</v>
       </c>
-      <c r="X3" s="12">
+      <c r="X3" s="10">
         <v>165.7</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Y3" s="10">
         <v>169.7</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="Z3" s="10">
         <v>176.5</v>
       </c>
       <c r="AA3" s="2">
@@ -1642,8 +1644,8 @@
         <v>156.5</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1706,19 +1708,19 @@
       <c r="U4" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="V4" s="12" t="s">
+      <c r="V4" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="W4" s="12" t="s">
+      <c r="W4" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="X4" s="12" t="s">
+      <c r="X4" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="Y4" s="12" t="s">
+      <c r="Y4" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="Z4" s="12" t="s">
+      <c r="Z4" s="10" t="s">
         <v>198</v>
       </c>
       <c r="AA4" s="2" t="s">
@@ -1737,8 +1739,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="33" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:31" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1799,19 +1801,19 @@
       <c r="U5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="V5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="W5" s="13" t="s">
+      <c r="W5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="X5" s="13" t="s">
+      <c r="X5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Y5" s="13" t="s">
+      <c r="Y5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Z5" s="13" t="s">
+      <c r="Z5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="AA5" s="3" t="s">
@@ -1830,8 +1832,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1894,19 +1896,19 @@
       <c r="U6" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="V6" s="12" t="s">
+      <c r="V6" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="W6" s="12" t="s">
+      <c r="W6" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="X6" s="12" t="s">
+      <c r="X6" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="Y6" s="12" t="s">
+      <c r="Y6" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="Z6" s="12" t="s">
+      <c r="Z6" s="10" t="s">
         <v>203</v>
       </c>
       <c r="AA6" s="2" t="s">
@@ -1925,8 +1927,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:31" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1987,19 +1989,19 @@
       <c r="U7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="V7" s="13" t="s">
+      <c r="V7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="X7" s="13" t="s">
+      <c r="X7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="Y7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="Z7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="AA7" s="3" t="s">
@@ -2018,42 +2020,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
     </row>
-    <row r="9" spans="1:31" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2117,19 +2119,19 @@
       <c r="U9" s="2">
         <v>117</v>
       </c>
-      <c r="V9" s="12">
+      <c r="V9" s="10">
         <v>142</v>
       </c>
-      <c r="W9" s="12">
+      <c r="W9" s="10">
         <v>130</v>
       </c>
-      <c r="X9" s="12">
+      <c r="X9" s="10">
         <v>123</v>
       </c>
-      <c r="Y9" s="12">
+      <c r="Y9" s="10">
         <v>129</v>
       </c>
-      <c r="Z9" s="12">
+      <c r="Z9" s="10">
         <v>129</v>
       </c>
       <c r="AA9" s="2">
@@ -2148,7 +2150,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -2212,19 +2214,19 @@
       <c r="U10" s="2">
         <v>81</v>
       </c>
-      <c r="V10" s="12">
+      <c r="V10" s="10">
         <v>109</v>
       </c>
-      <c r="W10" s="12">
+      <c r="W10" s="10">
         <v>97</v>
       </c>
-      <c r="X10" s="12">
+      <c r="X10" s="10">
         <v>75</v>
       </c>
-      <c r="Y10" s="12">
+      <c r="Y10" s="10">
         <v>100</v>
       </c>
-      <c r="Z10" s="12">
+      <c r="Z10" s="10">
         <v>86</v>
       </c>
       <c r="AA10" s="2">
@@ -2243,7 +2245,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -2307,19 +2309,19 @@
       <c r="U11" s="2">
         <v>107</v>
       </c>
-      <c r="V11" s="12">
+      <c r="V11" s="10">
         <v>133</v>
       </c>
-      <c r="W11" s="12">
+      <c r="W11" s="10">
         <v>121</v>
       </c>
-      <c r="X11" s="12">
+      <c r="X11" s="10">
         <v>106</v>
       </c>
-      <c r="Y11" s="12">
+      <c r="Y11" s="10">
         <v>119</v>
       </c>
-      <c r="Z11" s="12">
+      <c r="Z11" s="10">
         <v>109</v>
       </c>
       <c r="AA11" s="2">
@@ -2338,7 +2340,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -2402,19 +2404,19 @@
       <c r="U12" s="2">
         <v>12.4</v>
       </c>
-      <c r="V12" s="12">
+      <c r="V12" s="10">
         <v>16.2</v>
       </c>
-      <c r="W12" s="12">
+      <c r="W12" s="10">
         <v>18.5</v>
       </c>
-      <c r="X12" s="12">
+      <c r="X12" s="10">
         <v>12.7</v>
       </c>
-      <c r="Y12" s="12">
+      <c r="Y12" s="10">
         <v>15.4</v>
       </c>
-      <c r="Z12" s="12">
+      <c r="Z12" s="10">
         <v>16</v>
       </c>
       <c r="AA12" s="2">
@@ -2433,42 +2435,42 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="6"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12"/>
     </row>
-    <row r="14" spans="1:31" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -2532,19 +2534,19 @@
       <c r="U14" s="2">
         <v>1421</v>
       </c>
-      <c r="V14" s="12">
+      <c r="V14" s="10">
         <v>2261</v>
       </c>
-      <c r="W14" s="12">
+      <c r="W14" s="10">
         <v>2072</v>
       </c>
-      <c r="X14" s="12">
+      <c r="X14" s="10">
         <v>1928</v>
       </c>
-      <c r="Y14" s="12">
+      <c r="Y14" s="10">
         <v>1598</v>
       </c>
-      <c r="Z14" s="12">
+      <c r="Z14" s="10">
         <v>1686</v>
       </c>
       <c r="AA14" s="2">
@@ -2563,7 +2565,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="117.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -2625,19 +2627,19 @@
       <c r="U15" s="2">
         <v>1.05</v>
       </c>
-      <c r="V15" s="12">
+      <c r="V15" s="10">
         <v>1.04</v>
       </c>
-      <c r="W15" s="12">
+      <c r="W15" s="10">
         <v>0.99</v>
       </c>
-      <c r="X15" s="12">
+      <c r="X15" s="10">
         <v>0.79</v>
       </c>
-      <c r="Y15" s="12">
+      <c r="Y15" s="10">
         <v>1.18</v>
       </c>
-      <c r="Z15" s="12">
+      <c r="Z15" s="10">
         <v>1.04</v>
       </c>
       <c r="AA15" s="2">
@@ -2656,7 +2658,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -2718,19 +2720,19 @@
       <c r="U16" s="2">
         <v>1487</v>
       </c>
-      <c r="V16" s="12">
+      <c r="V16" s="10">
         <v>2356</v>
       </c>
-      <c r="W16" s="12">
+      <c r="W16" s="10">
         <v>2052</v>
       </c>
-      <c r="X16" s="12">
+      <c r="X16" s="10">
         <v>1516</v>
       </c>
-      <c r="Y16" s="12">
+      <c r="Y16" s="10">
         <v>1878</v>
       </c>
-      <c r="Z16" s="12">
+      <c r="Z16" s="10">
         <v>1760</v>
       </c>
       <c r="AA16" s="2">
@@ -2749,42 +2751,42 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="12"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="12"/>
     </row>
-    <row r="18" spans="1:31" ht="99" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -2848,19 +2850,19 @@
       <c r="U18" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="V18" s="12" t="s">
+      <c r="V18" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="W18" s="12" t="s">
+      <c r="W18" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="X18" s="12" t="s">
+      <c r="X18" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="Y18" s="12" t="s">
+      <c r="Y18" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="Z18" s="12" t="s">
+      <c r="Z18" s="10" t="s">
         <v>208</v>
       </c>
       <c r="AA18" s="2" t="s">
@@ -2879,7 +2881,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="99" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -2943,19 +2945,19 @@
       <c r="U19" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="V19" s="12" t="s">
+      <c r="V19" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="W19" s="12" t="s">
+      <c r="W19" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="X19" s="12" t="s">
+      <c r="X19" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="Y19" s="12" t="s">
+      <c r="Y19" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="Z19" s="12" t="s">
+      <c r="Z19" s="10" t="s">
         <v>213</v>
       </c>
       <c r="AA19" s="2" t="s">
@@ -2974,7 +2976,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="132" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="134.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
@@ -3038,19 +3040,19 @@
       <c r="U20" s="2">
         <v>152</v>
       </c>
-      <c r="V20" s="12">
+      <c r="V20" s="10">
         <v>212</v>
       </c>
-      <c r="W20" s="12">
+      <c r="W20" s="10">
         <v>282</v>
       </c>
-      <c r="X20" s="12">
+      <c r="X20" s="10">
         <v>151</v>
       </c>
-      <c r="Y20" s="12">
+      <c r="Y20" s="10">
         <v>197</v>
       </c>
-      <c r="Z20" s="12">
+      <c r="Z20" s="10">
         <v>197</v>
       </c>
       <c r="AA20" s="2">
@@ -3069,7 +3071,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="132" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="134.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -3133,19 +3135,19 @@
       <c r="U21" s="2">
         <v>61</v>
       </c>
-      <c r="V21" s="12">
+      <c r="V21" s="10">
         <v>116</v>
       </c>
-      <c r="W21" s="12">
+      <c r="W21" s="10">
         <v>150</v>
       </c>
-      <c r="X21" s="12">
+      <c r="X21" s="10">
         <v>65</v>
       </c>
-      <c r="Y21" s="12">
+      <c r="Y21" s="10">
         <v>103</v>
       </c>
-      <c r="Z21" s="12">
+      <c r="Z21" s="10">
         <v>97</v>
       </c>
       <c r="AA21" s="2">
@@ -3164,42 +3166,42 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="14"/>
-      <c r="X22" s="14"/>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="14"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="12"/>
+      <c r="AD22" s="12"/>
+      <c r="AE22" s="12"/>
     </row>
-    <row r="23" spans="1:31" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
@@ -3261,19 +3263,19 @@
       <c r="U23" s="2">
         <v>56</v>
       </c>
-      <c r="V23" s="12">
+      <c r="V23" s="10">
         <v>62</v>
       </c>
-      <c r="W23" s="12">
+      <c r="W23" s="10">
         <v>56</v>
       </c>
-      <c r="X23" s="12">
+      <c r="X23" s="10">
         <v>44</v>
       </c>
-      <c r="Y23" s="12">
+      <c r="Y23" s="10">
         <v>57</v>
       </c>
-      <c r="Z23" s="12">
+      <c r="Z23" s="10">
         <v>51</v>
       </c>
       <c r="AA23" s="2">
@@ -3292,7 +3294,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="99" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -3354,19 +3356,19 @@
       <c r="U24" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="V24" s="12" t="s">
+      <c r="V24" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="W24" s="12" t="s">
+      <c r="W24" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="X24" s="12" t="s">
+      <c r="X24" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="Y24" s="12" t="s">
+      <c r="Y24" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="Z24" s="12" t="s">
+      <c r="Z24" s="10" t="s">
         <v>218</v>
       </c>
       <c r="AA24" s="2" t="s">
@@ -3385,7 +3387,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -3447,19 +3449,19 @@
       <c r="U25" s="2">
         <v>14</v>
       </c>
-      <c r="V25" s="12">
+      <c r="V25" s="10">
         <v>35</v>
       </c>
-      <c r="W25" s="12">
+      <c r="W25" s="10">
         <v>18</v>
       </c>
-      <c r="X25" s="12">
+      <c r="X25" s="10">
         <v>6</v>
       </c>
-      <c r="Y25" s="12">
+      <c r="Y25" s="10">
         <v>22</v>
       </c>
-      <c r="Z25" s="12">
+      <c r="Z25" s="10">
         <v>17</v>
       </c>
       <c r="AA25" s="2">
@@ -3478,7 +3480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="99" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -3540,19 +3542,19 @@
       <c r="U26" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="V26" s="12" t="s">
+      <c r="V26" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="W26" s="12" t="s">
+      <c r="W26" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="X26" s="12" t="s">
+      <c r="X26" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="Y26" s="12" t="s">
+      <c r="Y26" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="Z26" s="12" t="s">
+      <c r="Z26" s="10" t="s">
         <v>223</v>
       </c>
       <c r="AA26" s="2" t="s">
@@ -3571,42 +3573,42 @@
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="6"/>
-      <c r="AC27" s="6"/>
-      <c r="AD27" s="6"/>
-      <c r="AE27" s="6"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="12"/>
     </row>
-    <row r="28" spans="1:31" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="84" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -3668,19 +3670,19 @@
       <c r="U28" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V28" s="12" t="s">
+      <c r="V28" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="W28" s="12" t="s">
+      <c r="W28" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="X28" s="12" t="s">
+      <c r="X28" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="Y28" s="12" t="s">
+      <c r="Y28" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="Z28" s="12" t="s">
+      <c r="Z28" s="10" t="s">
         <v>228</v>
       </c>
       <c r="AA28" s="2" t="s">
@@ -3699,7 +3701,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="84" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
@@ -3761,19 +3763,19 @@
       <c r="U29" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="V29" s="12" t="s">
+      <c r="V29" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="W29" s="12" t="s">
+      <c r="W29" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="X29" s="12" t="s">
+      <c r="X29" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="Y29" s="12" t="s">
+      <c r="Y29" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="Z29" s="12" t="s">
+      <c r="Z29" s="10" t="s">
         <v>176</v>
       </c>
       <c r="AA29" s="2" t="s">
@@ -3792,7 +3794,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
@@ -3856,19 +3858,19 @@
       <c r="U30" s="2">
         <v>162</v>
       </c>
-      <c r="V30" s="12">
+      <c r="V30" s="10">
         <v>295</v>
       </c>
-      <c r="W30" s="12">
+      <c r="W30" s="10">
         <v>205</v>
       </c>
-      <c r="X30" s="12">
+      <c r="X30" s="10">
         <v>74</v>
       </c>
-      <c r="Y30" s="12">
+      <c r="Y30" s="10">
         <v>27</v>
       </c>
-      <c r="Z30" s="12">
+      <c r="Z30" s="10">
         <v>79</v>
       </c>
       <c r="AA30" s="2">
@@ -3887,7 +3889,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
@@ -3951,19 +3953,19 @@
       <c r="U31" s="2">
         <v>4</v>
       </c>
-      <c r="V31" s="12">
+      <c r="V31" s="10">
         <v>4</v>
       </c>
-      <c r="W31" s="12">
+      <c r="W31" s="10">
         <v>6</v>
       </c>
-      <c r="X31" s="12">
+      <c r="X31" s="10">
         <v>11</v>
       </c>
-      <c r="Y31" s="12">
+      <c r="Y31" s="10">
         <v>3</v>
       </c>
-      <c r="Z31" s="12">
+      <c r="Z31" s="10">
         <v>10</v>
       </c>
       <c r="AA31" s="2">
@@ -3982,7 +3984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
@@ -4044,19 +4046,19 @@
       <c r="U32" s="2">
         <v>10.6</v>
       </c>
-      <c r="V32" s="12">
+      <c r="V32" s="10">
         <v>10.5</v>
       </c>
-      <c r="W32" s="12">
+      <c r="W32" s="10">
         <v>7.6</v>
       </c>
-      <c r="X32" s="12">
+      <c r="X32" s="10">
         <v>9.9</v>
       </c>
-      <c r="Y32" s="12">
+      <c r="Y32" s="10">
         <v>8.9</v>
       </c>
-      <c r="Z32" s="12">
+      <c r="Z32" s="10">
         <v>9.8000000000000007</v>
       </c>
       <c r="AA32" s="2">
@@ -4075,7 +4077,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="66" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
@@ -4139,19 +4141,19 @@
       <c r="U33" s="2">
         <v>0.21</v>
       </c>
-      <c r="V33" s="12">
+      <c r="V33" s="10">
         <v>0.17</v>
       </c>
-      <c r="W33" s="12">
+      <c r="W33" s="10">
         <v>0.16</v>
       </c>
-      <c r="X33" s="12">
+      <c r="X33" s="10">
         <v>0.32</v>
       </c>
-      <c r="Y33" s="12">
+      <c r="Y33" s="10">
         <v>0.21</v>
       </c>
-      <c r="Z33" s="12">
+      <c r="Z33" s="10">
         <v>0.39</v>
       </c>
       <c r="AA33" s="2">
@@ -4172,6 +4174,28 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="L27:P27"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="Q13:U13"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="L17:P17"/>
+    <mergeCell ref="L22:P22"/>
     <mergeCell ref="AA17:AE17"/>
     <mergeCell ref="AA22:AE22"/>
     <mergeCell ref="AA27:AE27"/>
@@ -4182,34 +4206,21 @@
     <mergeCell ref="V27:Z27"/>
     <mergeCell ref="AA8:AE8"/>
     <mergeCell ref="AA13:AE13"/>
-    <mergeCell ref="L27:P27"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="Q13:U13"/>
-    <mergeCell ref="Q17:U17"/>
-    <mergeCell ref="Q22:U22"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="L17:P17"/>
-    <mergeCell ref="L22:P22"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A4728E04F1C25043A5F1733D73E0315E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6bd008f8564d3c14a12134b5f7cf3363">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="92d3c652-603a-41fa-8c9a-552c7b6a6b1a" xmlns:ns4="1bc0c355-0e38-4215-b729-fdd4cba65d21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12cf320a51b8067d9992c608eb861ccd" ns3:_="" ns4:_="">
     <xsd:import namespace="92d3c652-603a-41fa-8c9a-552c7b6a6b1a"/>
@@ -4410,15 +4421,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4428,6 +4430,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{186117A0-A976-486E-B18E-259D3F4D1858}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5B39C3-7A50-46A8-B2AE-0D5BEE5F0385}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4442,14 +4452,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{186117A0-A976-486E-B18E-259D3F4D1858}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>